<commit_message>
update nlex toll rates
</commit_message>
<xml_diff>
--- a/apps/matrix-importer/class1.xlsx
+++ b/apps/matrix-importer/class1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan.zoleta/Projects/toll-ph/apps/matrix-importer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211FB0D4-D804-DC40-8081-A985D1504A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3A770E-9156-CE46-B422-A13778987785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{4EA19FBD-5D92-6444-BD69-1DAF73CA6D21}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{4EA19FBD-5D92-6444-BD69-1DAF73CA6D21}"/>
   </bookViews>
   <sheets>
     <sheet name="SLEX_SKYWAY_MCX" sheetId="2" r:id="rId1"/>
+    <sheet name="NLEX_SCTEX" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>C-5</t>
   </si>
@@ -105,6 +106,102 @@
   </si>
   <si>
     <t>Magallanes (Skyway)</t>
+  </si>
+  <si>
+    <t>Mindanao Avenue</t>
+  </si>
+  <si>
+    <t>Karuhatan</t>
+  </si>
+  <si>
+    <t>Valenzuela</t>
+  </si>
+  <si>
+    <t>Meycauayan</t>
+  </si>
+  <si>
+    <t>Marilao</t>
+  </si>
+  <si>
+    <t>Ciudad de Victoria</t>
+  </si>
+  <si>
+    <t>Bocaue</t>
+  </si>
+  <si>
+    <t>Tambubong</t>
+  </si>
+  <si>
+    <t>Balagtas</t>
+  </si>
+  <si>
+    <t>Tabang</t>
+  </si>
+  <si>
+    <t>Sta. Rita</t>
+  </si>
+  <si>
+    <t>Pulilan</t>
+  </si>
+  <si>
+    <t>San Simon</t>
+  </si>
+  <si>
+    <t>San Fernando</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Angeles</t>
+  </si>
+  <si>
+    <t>Dau</t>
+  </si>
+  <si>
+    <t>Sta. Ines</t>
+  </si>
+  <si>
+    <t>Dinalupihan</t>
+  </si>
+  <si>
+    <t>Floridablanca</t>
+  </si>
+  <si>
+    <t>Porac</t>
+  </si>
+  <si>
+    <t>Clark South</t>
+  </si>
+  <si>
+    <t>Mabalacat (Mabiga)</t>
+  </si>
+  <si>
+    <t>Clark North</t>
+  </si>
+  <si>
+    <t>Dolores</t>
+  </si>
+  <si>
+    <t>Concepcion</t>
+  </si>
+  <si>
+    <t>Tarlac</t>
+  </si>
+  <si>
+    <t>Balintawak</t>
+  </si>
+  <si>
+    <t>Mindanao Ave.</t>
+  </si>
+  <si>
+    <t>Tipo/Subic</t>
+  </si>
+  <si>
+    <t>Bamban/New Clark City</t>
+  </si>
+  <si>
+    <t>Hacienda Luisita</t>
   </si>
 </sst>
 </file>
@@ -486,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946B9BC0-D3F5-9546-A306-F01AB88FB40B}">
   <dimension ref="A1:W68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -1664,4 +1761,1564 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD87AD6-77A5-4B4B-99F8-57403E0138FF}">
+  <dimension ref="A1:AD31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>85</v>
+      </c>
+      <c r="C4">
+        <v>85</v>
+      </c>
+      <c r="D4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>85</v>
+      </c>
+      <c r="C5">
+        <v>85</v>
+      </c>
+      <c r="D5">
+        <v>85</v>
+      </c>
+      <c r="E5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>85</v>
+      </c>
+      <c r="C6">
+        <v>85</v>
+      </c>
+      <c r="D6">
+        <v>85</v>
+      </c>
+      <c r="E6">
+        <v>85</v>
+      </c>
+      <c r="F6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>96</v>
+      </c>
+      <c r="C7">
+        <v>96</v>
+      </c>
+      <c r="D7">
+        <v>96</v>
+      </c>
+      <c r="E7">
+        <v>96</v>
+      </c>
+      <c r="F7">
+        <v>96</v>
+      </c>
+      <c r="G7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>105</v>
+      </c>
+      <c r="C8">
+        <v>105</v>
+      </c>
+      <c r="D8">
+        <v>105</v>
+      </c>
+      <c r="E8">
+        <v>105</v>
+      </c>
+      <c r="F8">
+        <v>105</v>
+      </c>
+      <c r="G8">
+        <v>105</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+      <c r="C9">
+        <v>110</v>
+      </c>
+      <c r="D9">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <v>110</v>
+      </c>
+      <c r="G9">
+        <v>110</v>
+      </c>
+      <c r="H9">
+        <v>14</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>136</v>
+      </c>
+      <c r="C10">
+        <v>136</v>
+      </c>
+      <c r="D10">
+        <v>136</v>
+      </c>
+      <c r="E10">
+        <v>136</v>
+      </c>
+      <c r="F10">
+        <v>136</v>
+      </c>
+      <c r="G10">
+        <v>136</v>
+      </c>
+      <c r="H10">
+        <v>40</v>
+      </c>
+      <c r="I10">
+        <v>31</v>
+      </c>
+      <c r="J10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>157</v>
+      </c>
+      <c r="C11">
+        <v>157</v>
+      </c>
+      <c r="D11">
+        <v>157</v>
+      </c>
+      <c r="E11">
+        <v>157</v>
+      </c>
+      <c r="F11">
+        <v>157</v>
+      </c>
+      <c r="G11">
+        <v>157</v>
+      </c>
+      <c r="H11">
+        <v>61</v>
+      </c>
+      <c r="I11">
+        <v>52</v>
+      </c>
+      <c r="J11">
+        <v>47</v>
+      </c>
+      <c r="K11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>164</v>
+      </c>
+      <c r="C12">
+        <v>164</v>
+      </c>
+      <c r="D12">
+        <v>164</v>
+      </c>
+      <c r="E12">
+        <v>164</v>
+      </c>
+      <c r="F12">
+        <v>164</v>
+      </c>
+      <c r="G12">
+        <v>164</v>
+      </c>
+      <c r="H12">
+        <v>68</v>
+      </c>
+      <c r="I12">
+        <v>59</v>
+      </c>
+      <c r="J12">
+        <v>54</v>
+      </c>
+      <c r="K12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>202</v>
+      </c>
+      <c r="C13">
+        <v>202</v>
+      </c>
+      <c r="D13">
+        <v>202</v>
+      </c>
+      <c r="E13">
+        <v>202</v>
+      </c>
+      <c r="F13">
+        <v>202</v>
+      </c>
+      <c r="G13">
+        <v>202</v>
+      </c>
+      <c r="H13">
+        <v>106</v>
+      </c>
+      <c r="I13">
+        <v>97</v>
+      </c>
+      <c r="J13">
+        <v>92</v>
+      </c>
+      <c r="K13">
+        <v>66</v>
+      </c>
+      <c r="L13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>266</v>
+      </c>
+      <c r="C14">
+        <v>266</v>
+      </c>
+      <c r="D14">
+        <v>266</v>
+      </c>
+      <c r="E14">
+        <v>266</v>
+      </c>
+      <c r="F14">
+        <v>266</v>
+      </c>
+      <c r="G14">
+        <v>266</v>
+      </c>
+      <c r="H14">
+        <v>170</v>
+      </c>
+      <c r="I14">
+        <v>160</v>
+      </c>
+      <c r="J14">
+        <v>155</v>
+      </c>
+      <c r="K14">
+        <v>130</v>
+      </c>
+      <c r="L14">
+        <v>101</v>
+      </c>
+      <c r="M14">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>314</v>
+      </c>
+      <c r="C15">
+        <v>314</v>
+      </c>
+      <c r="D15">
+        <v>314</v>
+      </c>
+      <c r="E15">
+        <v>314</v>
+      </c>
+      <c r="F15">
+        <v>314</v>
+      </c>
+      <c r="G15">
+        <v>314</v>
+      </c>
+      <c r="H15">
+        <v>218</v>
+      </c>
+      <c r="I15">
+        <v>209</v>
+      </c>
+      <c r="J15">
+        <v>204</v>
+      </c>
+      <c r="K15">
+        <v>178</v>
+      </c>
+      <c r="L15">
+        <v>150</v>
+      </c>
+      <c r="M15">
+        <v>113</v>
+      </c>
+      <c r="N15">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>353</v>
+      </c>
+      <c r="C16">
+        <v>353</v>
+      </c>
+      <c r="D16">
+        <v>353</v>
+      </c>
+      <c r="E16">
+        <v>353</v>
+      </c>
+      <c r="F16">
+        <v>353</v>
+      </c>
+      <c r="G16">
+        <v>353</v>
+      </c>
+      <c r="H16">
+        <v>257</v>
+      </c>
+      <c r="I16">
+        <v>248</v>
+      </c>
+      <c r="J16">
+        <v>243</v>
+      </c>
+      <c r="K16">
+        <v>217</v>
+      </c>
+      <c r="L16">
+        <v>189</v>
+      </c>
+      <c r="M16">
+        <v>151</v>
+      </c>
+      <c r="N16">
+        <v>87</v>
+      </c>
+      <c r="O16">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>399</v>
+      </c>
+      <c r="C17">
+        <v>399</v>
+      </c>
+      <c r="D17">
+        <v>399</v>
+      </c>
+      <c r="E17">
+        <v>399</v>
+      </c>
+      <c r="F17">
+        <v>399</v>
+      </c>
+      <c r="G17">
+        <v>399</v>
+      </c>
+      <c r="H17">
+        <v>303</v>
+      </c>
+      <c r="I17">
+        <v>294</v>
+      </c>
+      <c r="J17">
+        <v>289</v>
+      </c>
+      <c r="K17">
+        <v>263</v>
+      </c>
+      <c r="L17">
+        <v>235</v>
+      </c>
+      <c r="M17">
+        <v>198</v>
+      </c>
+      <c r="N17">
+        <v>134</v>
+      </c>
+      <c r="O17">
+        <v>85</v>
+      </c>
+      <c r="P17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>411</v>
+      </c>
+      <c r="C18">
+        <v>411</v>
+      </c>
+      <c r="D18">
+        <v>411</v>
+      </c>
+      <c r="E18">
+        <v>411</v>
+      </c>
+      <c r="F18">
+        <v>411</v>
+      </c>
+      <c r="G18">
+        <v>411</v>
+      </c>
+      <c r="H18">
+        <v>315</v>
+      </c>
+      <c r="I18">
+        <v>305</v>
+      </c>
+      <c r="J18">
+        <v>300</v>
+      </c>
+      <c r="K18">
+        <v>275</v>
+      </c>
+      <c r="L18">
+        <v>246</v>
+      </c>
+      <c r="M18">
+        <v>209</v>
+      </c>
+      <c r="N18">
+        <v>145</v>
+      </c>
+      <c r="O18">
+        <v>96</v>
+      </c>
+      <c r="P18">
+        <v>57</v>
+      </c>
+      <c r="Q18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>440</v>
+      </c>
+      <c r="C19">
+        <v>440</v>
+      </c>
+      <c r="D19">
+        <v>440</v>
+      </c>
+      <c r="E19">
+        <v>440</v>
+      </c>
+      <c r="F19">
+        <v>440</v>
+      </c>
+      <c r="G19">
+        <v>440</v>
+      </c>
+      <c r="H19">
+        <v>344</v>
+      </c>
+      <c r="I19">
+        <v>334</v>
+      </c>
+      <c r="J19">
+        <v>329</v>
+      </c>
+      <c r="K19">
+        <v>304</v>
+      </c>
+      <c r="L19">
+        <v>275</v>
+      </c>
+      <c r="M19">
+        <v>238</v>
+      </c>
+      <c r="N19">
+        <v>174</v>
+      </c>
+      <c r="O19">
+        <v>125</v>
+      </c>
+      <c r="P19">
+        <v>86</v>
+      </c>
+      <c r="Q19">
+        <v>40</v>
+      </c>
+      <c r="R19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>857</v>
+      </c>
+      <c r="C20">
+        <v>857</v>
+      </c>
+      <c r="D20">
+        <v>857</v>
+      </c>
+      <c r="E20">
+        <v>857</v>
+      </c>
+      <c r="F20">
+        <v>857</v>
+      </c>
+      <c r="G20">
+        <v>857</v>
+      </c>
+      <c r="H20">
+        <v>761</v>
+      </c>
+      <c r="I20">
+        <v>751</v>
+      </c>
+      <c r="J20">
+        <v>746</v>
+      </c>
+      <c r="K20">
+        <v>721</v>
+      </c>
+      <c r="L20">
+        <v>692</v>
+      </c>
+      <c r="M20">
+        <v>655</v>
+      </c>
+      <c r="N20">
+        <v>591</v>
+      </c>
+      <c r="O20">
+        <v>542</v>
+      </c>
+      <c r="P20">
+        <v>503</v>
+      </c>
+      <c r="Q20">
+        <v>457</v>
+      </c>
+      <c r="R20">
+        <v>446</v>
+      </c>
+      <c r="S20">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>731</v>
+      </c>
+      <c r="C21">
+        <v>731</v>
+      </c>
+      <c r="D21">
+        <v>731</v>
+      </c>
+      <c r="E21">
+        <v>731</v>
+      </c>
+      <c r="F21">
+        <v>731</v>
+      </c>
+      <c r="G21">
+        <v>731</v>
+      </c>
+      <c r="H21">
+        <v>635</v>
+      </c>
+      <c r="I21">
+        <v>625</v>
+      </c>
+      <c r="J21">
+        <v>620</v>
+      </c>
+      <c r="K21">
+        <v>595</v>
+      </c>
+      <c r="L21">
+        <v>566</v>
+      </c>
+      <c r="M21">
+        <v>529</v>
+      </c>
+      <c r="N21">
+        <v>465</v>
+      </c>
+      <c r="O21">
+        <v>416</v>
+      </c>
+      <c r="P21">
+        <v>377</v>
+      </c>
+      <c r="Q21">
+        <v>331</v>
+      </c>
+      <c r="R21">
+        <v>320</v>
+      </c>
+      <c r="S21">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22">
+        <v>608</v>
+      </c>
+      <c r="C22">
+        <v>608</v>
+      </c>
+      <c r="D22">
+        <v>608</v>
+      </c>
+      <c r="E22">
+        <v>608</v>
+      </c>
+      <c r="F22">
+        <v>608</v>
+      </c>
+      <c r="G22">
+        <v>608</v>
+      </c>
+      <c r="H22">
+        <v>512</v>
+      </c>
+      <c r="I22">
+        <v>502</v>
+      </c>
+      <c r="J22">
+        <v>497</v>
+      </c>
+      <c r="K22">
+        <v>472</v>
+      </c>
+      <c r="L22">
+        <v>443</v>
+      </c>
+      <c r="M22">
+        <v>406</v>
+      </c>
+      <c r="N22">
+        <v>342</v>
+      </c>
+      <c r="O22">
+        <v>293</v>
+      </c>
+      <c r="P22">
+        <v>254</v>
+      </c>
+      <c r="Q22">
+        <v>208</v>
+      </c>
+      <c r="R22">
+        <v>197</v>
+      </c>
+      <c r="S22">
+        <v>249</v>
+      </c>
+      <c r="T22">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <v>519</v>
+      </c>
+      <c r="C23">
+        <v>519</v>
+      </c>
+      <c r="D23">
+        <v>519</v>
+      </c>
+      <c r="E23">
+        <v>519</v>
+      </c>
+      <c r="F23">
+        <v>519</v>
+      </c>
+      <c r="G23">
+        <v>519</v>
+      </c>
+      <c r="H23">
+        <v>423</v>
+      </c>
+      <c r="I23">
+        <v>413</v>
+      </c>
+      <c r="J23">
+        <v>408</v>
+      </c>
+      <c r="K23">
+        <v>383</v>
+      </c>
+      <c r="L23">
+        <v>354</v>
+      </c>
+      <c r="M23">
+        <v>317</v>
+      </c>
+      <c r="N23">
+        <v>253</v>
+      </c>
+      <c r="O23">
+        <v>204</v>
+      </c>
+      <c r="P23">
+        <v>165</v>
+      </c>
+      <c r="Q23">
+        <v>119</v>
+      </c>
+      <c r="R23">
+        <v>108</v>
+      </c>
+      <c r="S23">
+        <v>339</v>
+      </c>
+      <c r="T23">
+        <v>213</v>
+      </c>
+      <c r="U23">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <v>451</v>
+      </c>
+      <c r="C24">
+        <v>451</v>
+      </c>
+      <c r="D24">
+        <v>451</v>
+      </c>
+      <c r="E24">
+        <v>451</v>
+      </c>
+      <c r="F24">
+        <v>451</v>
+      </c>
+      <c r="G24">
+        <v>451</v>
+      </c>
+      <c r="H24">
+        <v>355</v>
+      </c>
+      <c r="I24">
+        <v>345</v>
+      </c>
+      <c r="J24">
+        <v>340</v>
+      </c>
+      <c r="K24">
+        <v>315</v>
+      </c>
+      <c r="L24">
+        <v>286</v>
+      </c>
+      <c r="M24">
+        <v>249</v>
+      </c>
+      <c r="N24">
+        <v>185</v>
+      </c>
+      <c r="O24">
+        <v>136</v>
+      </c>
+      <c r="P24">
+        <v>97</v>
+      </c>
+      <c r="Q24">
+        <v>51</v>
+      </c>
+      <c r="R24">
+        <v>40</v>
+      </c>
+      <c r="S24">
+        <v>406</v>
+      </c>
+      <c r="T24">
+        <v>280</v>
+      </c>
+      <c r="U24">
+        <v>157</v>
+      </c>
+      <c r="V24">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>440</v>
+      </c>
+      <c r="C25">
+        <v>440</v>
+      </c>
+      <c r="D25">
+        <v>440</v>
+      </c>
+      <c r="E25">
+        <v>440</v>
+      </c>
+      <c r="F25">
+        <v>440</v>
+      </c>
+      <c r="G25">
+        <v>440</v>
+      </c>
+      <c r="H25">
+        <v>344</v>
+      </c>
+      <c r="I25">
+        <v>334</v>
+      </c>
+      <c r="J25">
+        <v>329</v>
+      </c>
+      <c r="K25">
+        <v>304</v>
+      </c>
+      <c r="L25">
+        <v>275</v>
+      </c>
+      <c r="M25">
+        <v>238</v>
+      </c>
+      <c r="N25">
+        <v>174</v>
+      </c>
+      <c r="O25">
+        <v>125</v>
+      </c>
+      <c r="P25">
+        <v>86</v>
+      </c>
+      <c r="Q25">
+        <v>40</v>
+      </c>
+      <c r="R25">
+        <v>29</v>
+      </c>
+      <c r="S25">
+        <v>417</v>
+      </c>
+      <c r="T25">
+        <v>291</v>
+      </c>
+      <c r="U25">
+        <v>168</v>
+      </c>
+      <c r="V25">
+        <v>79</v>
+      </c>
+      <c r="W25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26">
+        <v>467</v>
+      </c>
+      <c r="C26">
+        <v>467</v>
+      </c>
+      <c r="D26">
+        <v>467</v>
+      </c>
+      <c r="E26">
+        <v>467</v>
+      </c>
+      <c r="F26">
+        <v>467</v>
+      </c>
+      <c r="G26">
+        <v>467</v>
+      </c>
+      <c r="H26">
+        <v>371</v>
+      </c>
+      <c r="I26">
+        <v>361</v>
+      </c>
+      <c r="J26">
+        <v>356</v>
+      </c>
+      <c r="K26">
+        <v>331</v>
+      </c>
+      <c r="L26">
+        <v>302</v>
+      </c>
+      <c r="M26">
+        <v>265</v>
+      </c>
+      <c r="N26">
+        <v>201</v>
+      </c>
+      <c r="O26">
+        <v>152</v>
+      </c>
+      <c r="P26">
+        <v>113</v>
+      </c>
+      <c r="Q26">
+        <v>67</v>
+      </c>
+      <c r="R26">
+        <v>56</v>
+      </c>
+      <c r="S26">
+        <v>444</v>
+      </c>
+      <c r="T26">
+        <v>318</v>
+      </c>
+      <c r="U26">
+        <v>196</v>
+      </c>
+      <c r="V26">
+        <v>106</v>
+      </c>
+      <c r="W26">
+        <v>38</v>
+      </c>
+      <c r="X26">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>477</v>
+      </c>
+      <c r="C27">
+        <v>477</v>
+      </c>
+      <c r="D27">
+        <v>477</v>
+      </c>
+      <c r="E27">
+        <v>477</v>
+      </c>
+      <c r="F27">
+        <v>477</v>
+      </c>
+      <c r="G27">
+        <v>477</v>
+      </c>
+      <c r="H27">
+        <v>381</v>
+      </c>
+      <c r="I27">
+        <v>371</v>
+      </c>
+      <c r="J27">
+        <v>366</v>
+      </c>
+      <c r="K27">
+        <v>341</v>
+      </c>
+      <c r="L27">
+        <v>312</v>
+      </c>
+      <c r="M27">
+        <v>275</v>
+      </c>
+      <c r="N27">
+        <v>211</v>
+      </c>
+      <c r="O27">
+        <v>162</v>
+      </c>
+      <c r="P27">
+        <v>123</v>
+      </c>
+      <c r="Q27">
+        <v>77</v>
+      </c>
+      <c r="R27">
+        <v>66</v>
+      </c>
+      <c r="S27">
+        <v>454</v>
+      </c>
+      <c r="T27">
+        <v>328</v>
+      </c>
+      <c r="U27">
+        <v>206</v>
+      </c>
+      <c r="V27">
+        <v>116</v>
+      </c>
+      <c r="W27">
+        <v>48</v>
+      </c>
+      <c r="X27">
+        <v>37</v>
+      </c>
+      <c r="Y27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28">
+        <v>521</v>
+      </c>
+      <c r="C28">
+        <v>521</v>
+      </c>
+      <c r="D28">
+        <v>521</v>
+      </c>
+      <c r="E28">
+        <v>521</v>
+      </c>
+      <c r="F28">
+        <v>521</v>
+      </c>
+      <c r="G28">
+        <v>521</v>
+      </c>
+      <c r="H28">
+        <v>425</v>
+      </c>
+      <c r="I28">
+        <v>415</v>
+      </c>
+      <c r="J28">
+        <v>410</v>
+      </c>
+      <c r="K28">
+        <v>385</v>
+      </c>
+      <c r="L28">
+        <v>356</v>
+      </c>
+      <c r="M28">
+        <v>319</v>
+      </c>
+      <c r="N28">
+        <v>255</v>
+      </c>
+      <c r="O28">
+        <v>206</v>
+      </c>
+      <c r="P28">
+        <v>167</v>
+      </c>
+      <c r="Q28">
+        <v>121</v>
+      </c>
+      <c r="R28">
+        <v>110</v>
+      </c>
+      <c r="S28">
+        <v>498</v>
+      </c>
+      <c r="T28">
+        <v>372</v>
+      </c>
+      <c r="U28">
+        <v>249</v>
+      </c>
+      <c r="V28">
+        <v>159</v>
+      </c>
+      <c r="W28">
+        <v>92</v>
+      </c>
+      <c r="X28">
+        <v>81</v>
+      </c>
+      <c r="Y28">
+        <v>54</v>
+      </c>
+      <c r="Z28">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29">
+        <v>545</v>
+      </c>
+      <c r="C29">
+        <v>545</v>
+      </c>
+      <c r="D29">
+        <v>545</v>
+      </c>
+      <c r="E29">
+        <v>545</v>
+      </c>
+      <c r="F29">
+        <v>545</v>
+      </c>
+      <c r="G29">
+        <v>545</v>
+      </c>
+      <c r="H29">
+        <v>449</v>
+      </c>
+      <c r="I29">
+        <v>439</v>
+      </c>
+      <c r="J29">
+        <v>434</v>
+      </c>
+      <c r="K29">
+        <v>409</v>
+      </c>
+      <c r="L29">
+        <v>380</v>
+      </c>
+      <c r="M29">
+        <v>343</v>
+      </c>
+      <c r="N29">
+        <v>279</v>
+      </c>
+      <c r="O29">
+        <v>230</v>
+      </c>
+      <c r="P29">
+        <v>191</v>
+      </c>
+      <c r="Q29">
+        <v>145</v>
+      </c>
+      <c r="R29">
+        <v>134</v>
+      </c>
+      <c r="S29">
+        <v>523</v>
+      </c>
+      <c r="T29">
+        <v>397</v>
+      </c>
+      <c r="U29">
+        <v>274</v>
+      </c>
+      <c r="V29">
+        <v>184</v>
+      </c>
+      <c r="W29">
+        <v>116</v>
+      </c>
+      <c r="X29">
+        <v>105</v>
+      </c>
+      <c r="Y29">
+        <v>78</v>
+      </c>
+      <c r="Z29">
+        <v>68</v>
+      </c>
+      <c r="AA29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30">
+        <v>638</v>
+      </c>
+      <c r="C30">
+        <v>638</v>
+      </c>
+      <c r="D30">
+        <v>638</v>
+      </c>
+      <c r="E30">
+        <v>638</v>
+      </c>
+      <c r="F30">
+        <v>638</v>
+      </c>
+      <c r="G30">
+        <v>638</v>
+      </c>
+      <c r="H30">
+        <v>542</v>
+      </c>
+      <c r="I30">
+        <v>532</v>
+      </c>
+      <c r="J30">
+        <v>527</v>
+      </c>
+      <c r="K30">
+        <v>502</v>
+      </c>
+      <c r="L30">
+        <v>473</v>
+      </c>
+      <c r="M30">
+        <v>436</v>
+      </c>
+      <c r="N30">
+        <v>372</v>
+      </c>
+      <c r="O30">
+        <v>323</v>
+      </c>
+      <c r="P30">
+        <v>284</v>
+      </c>
+      <c r="Q30">
+        <v>238</v>
+      </c>
+      <c r="R30">
+        <v>227</v>
+      </c>
+      <c r="S30">
+        <v>615</v>
+      </c>
+      <c r="T30">
+        <v>489</v>
+      </c>
+      <c r="U30">
+        <v>366</v>
+      </c>
+      <c r="V30">
+        <v>276</v>
+      </c>
+      <c r="W30">
+        <v>209</v>
+      </c>
+      <c r="X30">
+        <v>198</v>
+      </c>
+      <c r="Y30">
+        <v>171</v>
+      </c>
+      <c r="Z30">
+        <v>160</v>
+      </c>
+      <c r="AA30">
+        <v>117</v>
+      </c>
+      <c r="AB30">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31">
+        <v>670</v>
+      </c>
+      <c r="C31">
+        <v>670</v>
+      </c>
+      <c r="D31">
+        <v>670</v>
+      </c>
+      <c r="E31">
+        <v>670</v>
+      </c>
+      <c r="F31">
+        <v>670</v>
+      </c>
+      <c r="G31">
+        <v>670</v>
+      </c>
+      <c r="H31">
+        <v>574</v>
+      </c>
+      <c r="I31">
+        <v>564</v>
+      </c>
+      <c r="J31">
+        <v>559</v>
+      </c>
+      <c r="K31">
+        <v>534</v>
+      </c>
+      <c r="L31">
+        <v>505</v>
+      </c>
+      <c r="M31">
+        <v>468</v>
+      </c>
+      <c r="N31">
+        <v>404</v>
+      </c>
+      <c r="O31">
+        <v>355</v>
+      </c>
+      <c r="P31">
+        <v>316</v>
+      </c>
+      <c r="Q31">
+        <v>270</v>
+      </c>
+      <c r="R31">
+        <v>259</v>
+      </c>
+      <c r="S31">
+        <v>647</v>
+      </c>
+      <c r="T31">
+        <v>521</v>
+      </c>
+      <c r="U31">
+        <v>398</v>
+      </c>
+      <c r="V31">
+        <v>308</v>
+      </c>
+      <c r="W31">
+        <v>241</v>
+      </c>
+      <c r="X31">
+        <v>230</v>
+      </c>
+      <c r="Y31">
+        <v>203</v>
+      </c>
+      <c r="Z31">
+        <v>193</v>
+      </c>
+      <c r="AA31">
+        <v>149</v>
+      </c>
+      <c r="AB31">
+        <v>124</v>
+      </c>
+      <c r="AC31">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>